<commit_message>
Removed leading spaces in Rainshelter Excel
</commit_message>
<xml_diff>
--- a/Tests/Validation/Ryegrass/RainShelter.xlsx
+++ b/Tests/Validation/Ryegrass/RainShelter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9AFC07-1260-495F-A942-9F2D521B7957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD95AA-E6B7-415E-9D84-7448518BC182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="81480" yWindow="15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-3975" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -514,28 +514,28 @@
     <t>22/05/2007</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soil.Output.SW(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soil.Output.SW(3)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Soil.Output.SW(4)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(5)</t>
+    <t>Soil.Output.SW(1)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(6)</t>
+    <t>Soil.Output.SW(2)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(7)</t>
+    <t>Soil.Output.SW(3)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(8)</t>
+    <t>Soil.Output.SW(5)</t>
+  </si>
+  <si>
+    <t>Soil.Output.SW(6)</t>
+  </si>
+  <si>
+    <t>Soil.Output.SW(7)</t>
+  </si>
+  <si>
+    <t>Soil.Output.SW(8)</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <dimension ref="A1:N797"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -929,16 +929,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Add Potential Potential Evaporation to Rainshelter
</commit_message>
<xml_diff>
--- a/Tests/Validation/Ryegrass/RainShelter.xlsx
+++ b/Tests/Validation/Ryegrass/RainShelter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD95AA-E6B7-415E-9D84-7448518BC182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A85B9D6-F22F-4D5A-A9CA-83F0765650F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-3975" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,9 +514,6 @@
     <t>22/05/2007</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soil.Output.SW(4)</t>
-  </si>
-  <si>
     <t>Soil.Output.SW(1)</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t>Soil.Output.SW(8)</t>
+  </si>
+  <si>
+    <t>Soil.Output.SW(4)</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <dimension ref="A1:N797"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -929,28 +929,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>

</xml_diff>